<commit_message>
Version pre-final de 2026
</commit_message>
<xml_diff>
--- a/BASE_PERSONNEL_.xlsx
+++ b/BASE_PERSONNEL_.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360281C2-4BE5-46E8-8987-F63FF46F0743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A6B5AA-7F89-4FC9-BDBA-19CCB3F8118C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12349" uniqueCount="3245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12507" uniqueCount="3245">
   <si>
     <t>AE</t>
   </si>
@@ -9853,13 +9853,6 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -9876,6 +9869,13 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
         </patternFill>
       </fill>
     </dxf>
@@ -10181,8 +10181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L1207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="A1197" workbookViewId="0">
+      <selection activeCell="D1205" sqref="D1205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10716,7 +10716,9 @@
       <c r="I14" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="J14" s="1"/>
+      <c r="J14" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K14" s="1" t="s">
         <v>91</v>
       </c>
@@ -11056,7 +11058,9 @@
       <c r="I23" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="J23" s="1"/>
+      <c r="J23" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K23" s="1" t="s">
         <v>91</v>
       </c>
@@ -11206,7 +11210,9 @@
       <c r="I27" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="J27" s="1"/>
+      <c r="J27" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K27" s="1" t="s">
         <v>91</v>
       </c>
@@ -11508,7 +11514,9 @@
       <c r="I35" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="J35" s="1"/>
+      <c r="J35" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K35" s="1" t="s">
         <v>91</v>
       </c>
@@ -30962,7 +30970,9 @@
       <c r="I547" s="1" t="s">
         <v>1397</v>
       </c>
-      <c r="J547" s="1"/>
+      <c r="J547" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K547" s="1" t="s">
         <v>91</v>
       </c>
@@ -31416,7 +31426,9 @@
       <c r="I559" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="J559" s="1"/>
+      <c r="J559" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K559" s="1" t="s">
         <v>91</v>
       </c>
@@ -31516,7 +31528,9 @@
       <c r="E562" s="1" t="s">
         <v>1488</v>
       </c>
-      <c r="F562" s="1"/>
+      <c r="F562" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="G562" s="1" t="s">
         <v>1448</v>
       </c>
@@ -31526,7 +31540,9 @@
       <c r="I562" s="1" t="s">
         <v>1489</v>
       </c>
-      <c r="J562" s="1"/>
+      <c r="J562" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K562" s="1" t="s">
         <v>91</v>
       </c>
@@ -31562,7 +31578,9 @@
       <c r="I563" s="1" t="s">
         <v>1494</v>
       </c>
-      <c r="J563" s="1"/>
+      <c r="J563" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K563" s="1" t="s">
         <v>91</v>
       </c>
@@ -31750,7 +31768,9 @@
       <c r="I568" s="1" t="s">
         <v>1513</v>
       </c>
-      <c r="J568" s="1"/>
+      <c r="J568" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K568" s="1" t="s">
         <v>91</v>
       </c>
@@ -31812,7 +31832,9 @@
       <c r="E570" s="1" t="s">
         <v>1488</v>
       </c>
-      <c r="F570" s="1"/>
+      <c r="F570" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="G570" s="1" t="s">
         <v>1448</v>
       </c>
@@ -31822,7 +31844,9 @@
       <c r="I570" s="1" t="s">
         <v>1489</v>
       </c>
-      <c r="J570" s="1"/>
+      <c r="J570" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K570" s="1" t="s">
         <v>91</v>
       </c>
@@ -31858,7 +31882,9 @@
       <c r="I571" s="1" t="s">
         <v>1520</v>
       </c>
-      <c r="J571" s="1"/>
+      <c r="J571" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K571" s="1" t="s">
         <v>91</v>
       </c>
@@ -31970,7 +31996,9 @@
       <c r="I574" s="1" t="s">
         <v>1527</v>
       </c>
-      <c r="J574" s="1"/>
+      <c r="J574" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K574" s="1" t="s">
         <v>91</v>
       </c>
@@ -32082,7 +32110,9 @@
       <c r="I577" s="1" t="s">
         <v>1537</v>
       </c>
-      <c r="J577" s="1"/>
+      <c r="J577" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K577" s="1" t="s">
         <v>91</v>
       </c>
@@ -32156,7 +32186,9 @@
       <c r="I579" s="1" t="s">
         <v>1544</v>
       </c>
-      <c r="J579" s="1"/>
+      <c r="J579" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K579" s="1" t="s">
         <v>91</v>
       </c>
@@ -32192,7 +32224,9 @@
       <c r="I580" s="1" t="s">
         <v>1547</v>
       </c>
-      <c r="J580" s="1"/>
+      <c r="J580" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K580" s="1" t="s">
         <v>91</v>
       </c>
@@ -32266,7 +32300,9 @@
       <c r="I582" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="J582" s="1"/>
+      <c r="J582" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K582" s="1" t="s">
         <v>91</v>
       </c>
@@ -32340,7 +32376,9 @@
       <c r="I584" s="1" t="s">
         <v>1561</v>
       </c>
-      <c r="J584" s="1"/>
+      <c r="J584" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K584" s="1" t="s">
         <v>91</v>
       </c>
@@ -32452,7 +32490,9 @@
       <c r="I587" s="1" t="s">
         <v>1571</v>
       </c>
-      <c r="J587" s="1"/>
+      <c r="J587" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K587" s="1" t="s">
         <v>91</v>
       </c>
@@ -32488,7 +32528,9 @@
       <c r="I588" s="1" t="s">
         <v>1573</v>
       </c>
-      <c r="J588" s="1"/>
+      <c r="J588" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K588" s="1" t="s">
         <v>91</v>
       </c>
@@ -32562,7 +32604,9 @@
       <c r="I590" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J590" s="1"/>
+      <c r="J590" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K590" s="1" t="s">
         <v>91</v>
       </c>
@@ -32636,7 +32680,9 @@
       <c r="I592" s="1" t="s">
         <v>1585</v>
       </c>
-      <c r="J592" s="1"/>
+      <c r="J592" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K592" s="1" t="s">
         <v>91</v>
       </c>
@@ -32710,7 +32756,9 @@
       <c r="I594" s="1" t="s">
         <v>1594</v>
       </c>
-      <c r="J594" s="1"/>
+      <c r="J594" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K594" s="1" t="s">
         <v>91</v>
       </c>
@@ -32746,7 +32794,9 @@
       <c r="I595" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="J595" s="1"/>
+      <c r="J595" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K595" s="1" t="s">
         <v>91</v>
       </c>
@@ -32820,7 +32870,9 @@
       <c r="I597" s="1" t="s">
         <v>1602</v>
       </c>
-      <c r="J597" s="1"/>
+      <c r="J597" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K597" s="1" t="s">
         <v>91</v>
       </c>
@@ -32856,7 +32908,9 @@
       <c r="I598" s="1" t="s">
         <v>1605</v>
       </c>
-      <c r="J598" s="1"/>
+      <c r="J598" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K598" s="1" t="s">
         <v>91</v>
       </c>
@@ -32930,7 +32984,9 @@
       <c r="I600" s="1" t="s">
         <v>1610</v>
       </c>
-      <c r="J600" s="1"/>
+      <c r="J600" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K600" s="1" t="s">
         <v>91</v>
       </c>
@@ -32966,7 +33022,9 @@
       <c r="I601" s="1" t="s">
         <v>1613</v>
       </c>
-      <c r="J601" s="1"/>
+      <c r="J601" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K601" s="1" t="s">
         <v>91</v>
       </c>
@@ -33040,7 +33098,9 @@
       <c r="I603" s="1" t="s">
         <v>1620</v>
       </c>
-      <c r="J603" s="1"/>
+      <c r="J603" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K603" s="1" t="s">
         <v>91</v>
       </c>
@@ -33114,7 +33174,9 @@
       <c r="I605" s="1" t="s">
         <v>1626</v>
       </c>
-      <c r="J605" s="1"/>
+      <c r="J605" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K605" s="1" t="s">
         <v>91</v>
       </c>
@@ -33150,7 +33212,9 @@
       <c r="I606" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="J606" s="1"/>
+      <c r="J606" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K606" s="1" t="s">
         <v>91</v>
       </c>
@@ -33186,7 +33250,9 @@
       <c r="I607" s="1" t="s">
         <v>1631</v>
       </c>
-      <c r="J607" s="1"/>
+      <c r="J607" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K607" s="1" t="s">
         <v>91</v>
       </c>
@@ -33222,7 +33288,9 @@
       <c r="I608" s="1" t="s">
         <v>1634</v>
       </c>
-      <c r="J608" s="1"/>
+      <c r="J608" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K608" s="1" t="s">
         <v>91</v>
       </c>
@@ -33258,7 +33326,9 @@
       <c r="I609" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="J609" s="1"/>
+      <c r="J609" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K609" s="1" t="s">
         <v>91</v>
       </c>
@@ -33294,7 +33364,9 @@
       <c r="I610" s="1" t="s">
         <v>1640</v>
       </c>
-      <c r="J610" s="1"/>
+      <c r="J610" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K610" s="1" t="s">
         <v>91</v>
       </c>
@@ -33368,7 +33440,9 @@
       <c r="I612" s="1" t="s">
         <v>1645</v>
       </c>
-      <c r="J612" s="1"/>
+      <c r="J612" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K612" s="1" t="s">
         <v>91</v>
       </c>
@@ -33442,7 +33516,9 @@
       <c r="I614" s="1" t="s">
         <v>1653</v>
       </c>
-      <c r="J614" s="1"/>
+      <c r="J614" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K614" s="1" t="s">
         <v>91</v>
       </c>
@@ -33516,7 +33592,9 @@
       <c r="I616" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="J616" s="1"/>
+      <c r="J616" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K616" s="1" t="s">
         <v>91</v>
       </c>
@@ -33590,7 +33668,9 @@
       <c r="I618" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="J618" s="1"/>
+      <c r="J618" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K618" s="1" t="s">
         <v>91</v>
       </c>
@@ -33664,7 +33744,9 @@
       <c r="I620" s="1" t="s">
         <v>1671</v>
       </c>
-      <c r="J620" s="1"/>
+      <c r="J620" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K620" s="1" t="s">
         <v>91</v>
       </c>
@@ -33688,7 +33770,9 @@
       <c r="E621" s="1" t="s">
         <v>1673</v>
       </c>
-      <c r="F621" s="1"/>
+      <c r="F621" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="G621" s="1" t="s">
         <v>1674</v>
       </c>
@@ -33698,7 +33782,9 @@
       <c r="I621" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="J621" s="1"/>
+      <c r="J621" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K621" s="1" t="s">
         <v>91</v>
       </c>
@@ -33734,7 +33820,9 @@
       <c r="I622" s="1" t="s">
         <v>1676</v>
       </c>
-      <c r="J622" s="1"/>
+      <c r="J622" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K622" s="1" t="s">
         <v>91</v>
       </c>
@@ -33846,7 +33934,9 @@
       <c r="I625" s="1" t="s">
         <v>1681</v>
       </c>
-      <c r="J625" s="1"/>
+      <c r="J625" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K625" s="1" t="s">
         <v>91</v>
       </c>
@@ -34034,7 +34124,9 @@
       <c r="I630" s="1" t="s">
         <v>1694</v>
       </c>
-      <c r="J630" s="1"/>
+      <c r="J630" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K630" s="1" t="s">
         <v>91</v>
       </c>
@@ -34070,7 +34162,9 @@
       <c r="I631" s="1" t="s">
         <v>1634</v>
       </c>
-      <c r="J631" s="1"/>
+      <c r="J631" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K631" s="1" t="s">
         <v>91</v>
       </c>
@@ -34144,7 +34238,9 @@
       <c r="I633" s="1" t="s">
         <v>1702</v>
       </c>
-      <c r="J633" s="1"/>
+      <c r="J633" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K633" s="1" t="s">
         <v>91</v>
       </c>
@@ -34218,7 +34314,9 @@
       <c r="I635" s="1" t="s">
         <v>1707</v>
       </c>
-      <c r="J635" s="1"/>
+      <c r="J635" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K635" s="1" t="s">
         <v>91</v>
       </c>
@@ -34292,7 +34390,9 @@
       <c r="I637" s="1" t="s">
         <v>1713</v>
       </c>
-      <c r="J637" s="1"/>
+      <c r="J637" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K637" s="1" t="s">
         <v>91</v>
       </c>
@@ -34328,7 +34428,9 @@
       <c r="I638" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="J638" s="1"/>
+      <c r="J638" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K638" s="1" t="s">
         <v>91</v>
       </c>
@@ -34364,7 +34466,9 @@
       <c r="I639" s="1" t="s">
         <v>1716</v>
       </c>
-      <c r="J639" s="1"/>
+      <c r="J639" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K639" s="1" t="s">
         <v>91</v>
       </c>
@@ -34438,7 +34542,9 @@
       <c r="I641" s="1" t="s">
         <v>1444</v>
       </c>
-      <c r="J641" s="1"/>
+      <c r="J641" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K641" s="1" t="s">
         <v>91</v>
       </c>
@@ -34474,7 +34580,9 @@
       <c r="I642" s="1" t="s">
         <v>744</v>
       </c>
-      <c r="J642" s="1"/>
+      <c r="J642" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K642" s="1" t="s">
         <v>91</v>
       </c>
@@ -34548,7 +34656,9 @@
       <c r="I644" s="1" t="s">
         <v>1473</v>
       </c>
-      <c r="J644" s="1"/>
+      <c r="J644" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K644" s="1" t="s">
         <v>91</v>
       </c>
@@ -34610,7 +34720,9 @@
       <c r="E646" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="F646" s="1"/>
+      <c r="F646" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="G646" s="1" t="s">
         <v>1699</v>
       </c>
@@ -34620,7 +34732,9 @@
       <c r="I646" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="J646" s="1"/>
+      <c r="J646" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K646" s="1" t="s">
         <v>91</v>
       </c>
@@ -34656,7 +34770,9 @@
       <c r="I647" s="1" t="s">
         <v>1734</v>
       </c>
-      <c r="J647" s="1"/>
+      <c r="J647" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K647" s="1" t="s">
         <v>91</v>
       </c>
@@ -34806,7 +34922,9 @@
       <c r="I651" s="1" t="s">
         <v>1745</v>
       </c>
-      <c r="J651" s="1"/>
+      <c r="J651" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K651" s="1" t="s">
         <v>91</v>
       </c>
@@ -34956,7 +35074,9 @@
       <c r="I655" s="1" t="s">
         <v>1756</v>
       </c>
-      <c r="J655" s="1"/>
+      <c r="J655" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K655" s="1" t="s">
         <v>91</v>
       </c>
@@ -34992,7 +35112,9 @@
       <c r="I656" s="1" t="s">
         <v>1758</v>
       </c>
-      <c r="J656" s="1"/>
+      <c r="J656" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K656" s="1" t="s">
         <v>91</v>
       </c>
@@ -35066,7 +35188,9 @@
       <c r="I658" s="1" t="s">
         <v>1765</v>
       </c>
-      <c r="J658" s="1"/>
+      <c r="J658" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K658" s="1" t="s">
         <v>91</v>
       </c>
@@ -35102,7 +35226,9 @@
       <c r="I659" s="1" t="s">
         <v>1469</v>
       </c>
-      <c r="J659" s="1"/>
+      <c r="J659" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K659" s="1" t="s">
         <v>91</v>
       </c>
@@ -35328,7 +35454,9 @@
       <c r="I665" s="1" t="s">
         <v>1776</v>
       </c>
-      <c r="J665" s="1"/>
+      <c r="J665" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K665" s="1" t="s">
         <v>91</v>
       </c>
@@ -35478,7 +35606,9 @@
       <c r="I669" s="1" t="s">
         <v>1790</v>
       </c>
-      <c r="J669" s="1"/>
+      <c r="J669" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K669" s="1" t="s">
         <v>91</v>
       </c>
@@ -35552,7 +35682,9 @@
       <c r="I671" s="1" t="s">
         <v>1796</v>
       </c>
-      <c r="J671" s="1"/>
+      <c r="J671" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K671" s="1" t="s">
         <v>91</v>
       </c>
@@ -35626,7 +35758,9 @@
       <c r="I673" s="1" t="s">
         <v>1803</v>
       </c>
-      <c r="J673" s="1"/>
+      <c r="J673" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K673" s="1" t="s">
         <v>91</v>
       </c>
@@ -35700,7 +35834,9 @@
       <c r="I675" s="1" t="s">
         <v>1812</v>
       </c>
-      <c r="J675" s="1"/>
+      <c r="J675" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K675" s="1" t="s">
         <v>91</v>
       </c>
@@ -35774,7 +35910,9 @@
       <c r="I677" s="1" t="s">
         <v>1817</v>
       </c>
-      <c r="J677" s="1"/>
+      <c r="J677" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K677" s="1" t="s">
         <v>91</v>
       </c>
@@ -35848,7 +35986,9 @@
       <c r="I679" s="1" t="s">
         <v>1825</v>
       </c>
-      <c r="J679" s="1"/>
+      <c r="J679" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K679" s="1" t="s">
         <v>91</v>
       </c>
@@ -35922,7 +36062,9 @@
       <c r="I681" s="1" t="s">
         <v>1834</v>
       </c>
-      <c r="J681" s="1"/>
+      <c r="J681" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K681" s="1" t="s">
         <v>91</v>
       </c>
@@ -35996,7 +36138,9 @@
       <c r="I683" s="1" t="s">
         <v>1842</v>
       </c>
-      <c r="J683" s="1"/>
+      <c r="J683" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K683" s="1" t="s">
         <v>91</v>
       </c>
@@ -36070,7 +36214,9 @@
       <c r="I685" s="1" t="s">
         <v>1834</v>
       </c>
-      <c r="J685" s="1"/>
+      <c r="J685" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K685" s="1" t="s">
         <v>91</v>
       </c>
@@ -36106,7 +36252,9 @@
       <c r="I686" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="J686" s="1"/>
+      <c r="J686" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K686" s="1" t="s">
         <v>91</v>
       </c>
@@ -36218,7 +36366,9 @@
       <c r="I689" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J689" s="1"/>
+      <c r="J689" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K689" s="1" t="s">
         <v>91</v>
       </c>
@@ -36292,7 +36442,9 @@
       <c r="I691" s="1" t="s">
         <v>1866</v>
       </c>
-      <c r="J691" s="1"/>
+      <c r="J691" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K691" s="1" t="s">
         <v>91</v>
       </c>
@@ -36366,7 +36518,9 @@
       <c r="I693" s="1" t="s">
         <v>1876</v>
       </c>
-      <c r="J693" s="1"/>
+      <c r="J693" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K693" s="1" t="s">
         <v>91</v>
       </c>
@@ -36440,7 +36594,9 @@
       <c r="I695" s="1" t="s">
         <v>1881</v>
       </c>
-      <c r="J695" s="1"/>
+      <c r="J695" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K695" s="1" t="s">
         <v>91</v>
       </c>
@@ -36476,7 +36632,9 @@
       <c r="I696" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="J696" s="1"/>
+      <c r="J696" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K696" s="1" t="s">
         <v>91</v>
       </c>
@@ -36512,7 +36670,9 @@
       <c r="I697" s="1" t="s">
         <v>1887</v>
       </c>
-      <c r="J697" s="1"/>
+      <c r="J697" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K697" s="1" t="s">
         <v>91</v>
       </c>
@@ -36548,7 +36708,9 @@
       <c r="I698" s="1" t="s">
         <v>1890</v>
       </c>
-      <c r="J698" s="1"/>
+      <c r="J698" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K698" s="1" t="s">
         <v>91</v>
       </c>
@@ -36584,7 +36746,9 @@
       <c r="I699" s="1" t="s">
         <v>1892</v>
       </c>
-      <c r="J699" s="1"/>
+      <c r="J699" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K699" s="1" t="s">
         <v>91</v>
       </c>
@@ -36620,7 +36784,9 @@
       <c r="I700" s="1" t="s">
         <v>1896</v>
       </c>
-      <c r="J700" s="1"/>
+      <c r="J700" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K700" s="1" t="s">
         <v>91</v>
       </c>
@@ -36682,7 +36848,9 @@
       <c r="E702" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F702" s="1"/>
+      <c r="F702" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="G702" s="1" t="s">
         <v>1737</v>
       </c>
@@ -36768,7 +36936,9 @@
       <c r="I704" s="1" t="s">
         <v>1904</v>
       </c>
-      <c r="J704" s="1"/>
+      <c r="J704" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K704" s="1" t="s">
         <v>91</v>
       </c>
@@ -36880,7 +37050,9 @@
       <c r="I707" s="1" t="s">
         <v>1910</v>
       </c>
-      <c r="J707" s="1"/>
+      <c r="J707" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K707" s="1" t="s">
         <v>91</v>
       </c>
@@ -36954,7 +37126,9 @@
       <c r="I709" s="1" t="s">
         <v>1834</v>
       </c>
-      <c r="J709" s="1"/>
+      <c r="J709" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K709" s="1" t="s">
         <v>91</v>
       </c>
@@ -36990,7 +37164,9 @@
       <c r="I710" s="1" t="s">
         <v>1918</v>
       </c>
-      <c r="J710" s="1"/>
+      <c r="J710" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K710" s="1" t="s">
         <v>91</v>
       </c>
@@ -37064,7 +37240,9 @@
       <c r="I712" s="1" t="s">
         <v>1925</v>
       </c>
-      <c r="J712" s="1"/>
+      <c r="J712" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K712" s="1" t="s">
         <v>91</v>
       </c>
@@ -37100,7 +37278,9 @@
       <c r="I713" s="1" t="s">
         <v>1928</v>
       </c>
-      <c r="J713" s="1"/>
+      <c r="J713" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K713" s="1" t="s">
         <v>91</v>
       </c>
@@ -37174,7 +37354,9 @@
       <c r="I715" s="1" t="s">
         <v>1935</v>
       </c>
-      <c r="J715" s="1"/>
+      <c r="J715" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K715" s="1" t="s">
         <v>91</v>
       </c>
@@ -37210,7 +37392,9 @@
       <c r="I716" s="1" t="s">
         <v>1938</v>
       </c>
-      <c r="J716" s="1"/>
+      <c r="J716" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K716" s="1" t="s">
         <v>91</v>
       </c>
@@ -37284,7 +37468,9 @@
       <c r="I718" s="1" t="s">
         <v>1944</v>
       </c>
-      <c r="J718" s="1"/>
+      <c r="J718" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K718" s="1" t="s">
         <v>91</v>
       </c>
@@ -37358,7 +37544,9 @@
       <c r="I720" s="1" t="s">
         <v>1948</v>
       </c>
-      <c r="J720" s="1"/>
+      <c r="J720" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K720" s="1" t="s">
         <v>91</v>
       </c>
@@ -37394,7 +37582,9 @@
       <c r="I721" s="1" t="s">
         <v>1951</v>
       </c>
-      <c r="J721" s="1"/>
+      <c r="J721" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K721" s="1" t="s">
         <v>91</v>
       </c>
@@ -37456,7 +37646,9 @@
       <c r="E723" s="1" t="s">
         <v>1954</v>
       </c>
-      <c r="F723" s="1"/>
+      <c r="F723" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="G723" s="1" t="s">
         <v>1678</v>
       </c>
@@ -37542,7 +37734,9 @@
       <c r="I725" s="1" t="s">
         <v>1963</v>
       </c>
-      <c r="J725" s="1"/>
+      <c r="J725" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K725" s="1" t="s">
         <v>91</v>
       </c>
@@ -37578,7 +37772,9 @@
       <c r="I726" s="1" t="s">
         <v>3243</v>
       </c>
-      <c r="J726" s="1"/>
+      <c r="J726" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K726" s="1" t="s">
         <v>91</v>
       </c>
@@ -37690,7 +37886,9 @@
       <c r="I729" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="J729" s="1"/>
+      <c r="J729" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K729" s="1" t="s">
         <v>91</v>
       </c>
@@ -37714,7 +37912,9 @@
       <c r="E730" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F730" s="1"/>
+      <c r="F730" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="G730" s="1" t="s">
         <v>1972</v>
       </c>
@@ -37724,7 +37924,9 @@
       <c r="I730" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="J730" s="1"/>
+      <c r="J730" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K730" s="1" t="s">
         <v>91</v>
       </c>
@@ -37760,7 +37962,9 @@
       <c r="I731" s="1" t="s">
         <v>1974</v>
       </c>
-      <c r="J731" s="1"/>
+      <c r="J731" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K731" s="1" t="s">
         <v>91</v>
       </c>
@@ -37834,7 +38038,9 @@
       <c r="I733" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J733" s="1"/>
+      <c r="J733" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K733" s="1" t="s">
         <v>91</v>
       </c>
@@ -37946,7 +38152,9 @@
       <c r="I736" s="1" t="s">
         <v>1986</v>
       </c>
-      <c r="J736" s="1"/>
+      <c r="J736" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K736" s="1" t="s">
         <v>91</v>
       </c>
@@ -41212,7 +41420,9 @@
       <c r="I822" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="J822" s="1"/>
+      <c r="J822" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K822" s="1" t="s">
         <v>91</v>
       </c>
@@ -41236,7 +41446,9 @@
       <c r="E823" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F823" s="1"/>
+      <c r="F823" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="G823" s="1" t="s">
         <v>2171</v>
       </c>
@@ -41284,7 +41496,9 @@
       <c r="I824" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J824" s="1"/>
+      <c r="J824" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K824" s="1" t="s">
         <v>91</v>
       </c>
@@ -41320,7 +41534,9 @@
       <c r="I825" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="J825" s="1"/>
+      <c r="J825" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K825" s="1" t="s">
         <v>91</v>
       </c>
@@ -41356,7 +41572,9 @@
       <c r="I826" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J826" s="1"/>
+      <c r="J826" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K826" s="1" t="s">
         <v>91</v>
       </c>
@@ -41392,7 +41610,9 @@
       <c r="I827" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="J827" s="1"/>
+      <c r="J827" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K827" s="1" t="s">
         <v>91</v>
       </c>
@@ -41428,7 +41648,9 @@
       <c r="I828" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J828" s="1"/>
+      <c r="J828" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K828" s="1" t="s">
         <v>91</v>
       </c>
@@ -41464,7 +41686,9 @@
       <c r="I829" s="1" t="s">
         <v>2242</v>
       </c>
-      <c r="J829" s="1"/>
+      <c r="J829" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K829" s="1" t="s">
         <v>91</v>
       </c>
@@ -41500,7 +41724,9 @@
       <c r="I830" s="1" t="s">
         <v>2246</v>
       </c>
-      <c r="J830" s="1"/>
+      <c r="J830" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K830" s="1" t="s">
         <v>91</v>
       </c>
@@ -41536,7 +41762,9 @@
       <c r="I831" s="1" t="s">
         <v>2250</v>
       </c>
-      <c r="J831" s="1"/>
+      <c r="J831" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K831" s="1" t="s">
         <v>91</v>
       </c>
@@ -41572,7 +41800,9 @@
       <c r="I832" s="1" t="s">
         <v>2253</v>
       </c>
-      <c r="J832" s="1"/>
+      <c r="J832" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K832" s="1" t="s">
         <v>91</v>
       </c>
@@ -41608,7 +41838,9 @@
       <c r="I833" s="1" t="s">
         <v>2257</v>
       </c>
-      <c r="J833" s="1"/>
+      <c r="J833" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K833" s="1" t="s">
         <v>91</v>
       </c>
@@ -41644,7 +41876,9 @@
       <c r="I834" s="1" t="s">
         <v>2259</v>
       </c>
-      <c r="J834" s="1"/>
+      <c r="J834" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K834" s="1" t="s">
         <v>91</v>
       </c>
@@ -41680,7 +41914,9 @@
       <c r="I835" s="1" t="s">
         <v>2262</v>
       </c>
-      <c r="J835" s="1"/>
+      <c r="J835" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K835" s="1" t="s">
         <v>91</v>
       </c>
@@ -41716,7 +41952,9 @@
       <c r="I836" s="1" t="s">
         <v>2266</v>
       </c>
-      <c r="J836" s="1"/>
+      <c r="J836" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K836" s="1" t="s">
         <v>91</v>
       </c>
@@ -41752,7 +41990,9 @@
       <c r="I837" s="1" t="s">
         <v>2269</v>
       </c>
-      <c r="J837" s="1"/>
+      <c r="J837" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K837" s="1" t="s">
         <v>91</v>
       </c>
@@ -41788,7 +42028,9 @@
       <c r="I838" s="1" t="s">
         <v>2271</v>
       </c>
-      <c r="J838" s="1"/>
+      <c r="J838" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K838" s="1" t="s">
         <v>91</v>
       </c>
@@ -41824,7 +42066,9 @@
       <c r="I839" s="1" t="s">
         <v>2273</v>
       </c>
-      <c r="J839" s="1"/>
+      <c r="J839" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K839" s="1" t="s">
         <v>91</v>
       </c>
@@ -41860,7 +42104,9 @@
       <c r="I840" s="1" t="s">
         <v>2277</v>
       </c>
-      <c r="J840" s="1"/>
+      <c r="J840" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K840" s="1" t="s">
         <v>91</v>
       </c>
@@ -41896,7 +42142,9 @@
       <c r="I841" s="1" t="s">
         <v>2280</v>
       </c>
-      <c r="J841" s="1"/>
+      <c r="J841" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K841" s="1" t="s">
         <v>91</v>
       </c>
@@ -41932,7 +42180,9 @@
       <c r="I842" s="1" t="s">
         <v>2284</v>
       </c>
-      <c r="J842" s="1"/>
+      <c r="J842" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K842" s="1" t="s">
         <v>91</v>
       </c>
@@ -41968,7 +42218,9 @@
       <c r="I843" s="1" t="s">
         <v>2288</v>
       </c>
-      <c r="J843" s="1"/>
+      <c r="J843" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K843" s="1" t="s">
         <v>91</v>
       </c>
@@ -42004,7 +42256,9 @@
       <c r="I844" s="1" t="s">
         <v>2293</v>
       </c>
-      <c r="J844" s="1"/>
+      <c r="J844" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K844" s="1" t="s">
         <v>91</v>
       </c>
@@ -42040,7 +42294,9 @@
       <c r="I845" s="1" t="s">
         <v>2296</v>
       </c>
-      <c r="J845" s="1"/>
+      <c r="J845" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K845" s="1" t="s">
         <v>91</v>
       </c>
@@ -42076,7 +42332,9 @@
       <c r="I846" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="J846" s="1"/>
+      <c r="J846" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K846" s="1" t="s">
         <v>91</v>
       </c>
@@ -42112,7 +42370,9 @@
       <c r="I847" s="1" t="s">
         <v>2302</v>
       </c>
-      <c r="J847" s="1"/>
+      <c r="J847" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K847" s="1" t="s">
         <v>91</v>
       </c>
@@ -42148,7 +42408,9 @@
       <c r="I848" s="1" t="s">
         <v>2306</v>
       </c>
-      <c r="J848" s="1"/>
+      <c r="J848" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K848" s="1" t="s">
         <v>91</v>
       </c>
@@ -42488,7 +42750,9 @@
       <c r="I857" s="1" t="s">
         <v>2330</v>
       </c>
-      <c r="J857" s="1"/>
+      <c r="J857" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K857" s="1" t="s">
         <v>91</v>
       </c>
@@ -42562,7 +42826,9 @@
       <c r="I859" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="J859" s="1"/>
+      <c r="J859" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K859" s="1" t="s">
         <v>91</v>
       </c>
@@ -42598,7 +42864,9 @@
       <c r="I860" s="1" t="s">
         <v>2337</v>
       </c>
-      <c r="J860" s="1"/>
+      <c r="J860" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K860" s="1" t="s">
         <v>91</v>
       </c>
@@ -42672,7 +42940,9 @@
       <c r="I862" s="1" t="s">
         <v>2344</v>
       </c>
-      <c r="J862" s="1"/>
+      <c r="J862" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K862" s="1" t="s">
         <v>91</v>
       </c>
@@ -42746,7 +43016,9 @@
       <c r="I864" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="J864" s="1"/>
+      <c r="J864" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K864" s="1" t="s">
         <v>91</v>
       </c>
@@ -42858,7 +43130,9 @@
       <c r="I867" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="J867" s="1"/>
+      <c r="J867" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K867" s="1" t="s">
         <v>91</v>
       </c>
@@ -43008,7 +43282,9 @@
       <c r="I871" s="1" t="s">
         <v>2365</v>
       </c>
-      <c r="J871" s="1"/>
+      <c r="J871" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K871" s="1" t="s">
         <v>91</v>
       </c>
@@ -43386,7 +43662,9 @@
       <c r="I881" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="J881" s="1"/>
+      <c r="J881" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K881" s="1" t="s">
         <v>91</v>
       </c>
@@ -43498,7 +43776,9 @@
       <c r="I884" s="1" t="s">
         <v>2403</v>
       </c>
-      <c r="J884" s="1"/>
+      <c r="J884" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K884" s="1" t="s">
         <v>91</v>
       </c>
@@ -43572,7 +43852,9 @@
       <c r="I886" s="1" t="s">
         <v>2405</v>
       </c>
-      <c r="J886" s="1"/>
+      <c r="J886" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K886" s="1" t="s">
         <v>91</v>
       </c>
@@ -43836,7 +44118,9 @@
       <c r="I893" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="J893" s="1"/>
+      <c r="J893" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K893" s="1" t="s">
         <v>91</v>
       </c>
@@ -43948,7 +44232,9 @@
       <c r="I896" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J896" s="1"/>
+      <c r="J896" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K896" s="1" t="s">
         <v>91</v>
       </c>
@@ -45656,7 +45942,9 @@
       <c r="I941" s="1" t="s">
         <v>2540</v>
       </c>
-      <c r="J941" s="1"/>
+      <c r="J941" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K941" s="1" t="s">
         <v>91</v>
       </c>
@@ -46528,7 +46816,9 @@
       <c r="I964" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="J964" s="1"/>
+      <c r="J964" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K964" s="1" t="s">
         <v>91</v>
       </c>
@@ -46754,7 +47044,9 @@
       <c r="I970" s="1" t="s">
         <v>2647</v>
       </c>
-      <c r="J970" s="1"/>
+      <c r="J970" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K970" s="1" t="s">
         <v>91</v>
       </c>
@@ -46828,7 +47120,9 @@
       <c r="I972" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="J972" s="1"/>
+      <c r="J972" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K972" s="1" t="s">
         <v>91</v>
       </c>
@@ -46864,7 +47158,9 @@
       <c r="I973" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="J973" s="1"/>
+      <c r="J973" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K973" s="1" t="s">
         <v>91</v>
       </c>
@@ -47318,7 +47614,9 @@
       <c r="I985" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="J985" s="1"/>
+      <c r="J985" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K985" s="1" t="s">
         <v>91</v>
       </c>
@@ -47810,7 +48108,9 @@
       <c r="I998" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="J998" s="1"/>
+      <c r="J998" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K998" s="1" t="s">
         <v>91</v>
       </c>
@@ -47846,7 +48146,9 @@
       <c r="I999" s="1" t="s">
         <v>2728</v>
       </c>
-      <c r="J999" s="1"/>
+      <c r="J999" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K999" s="1" t="s">
         <v>91</v>
       </c>
@@ -49592,7 +49894,9 @@
       <c r="I1045" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="J1045" s="1"/>
+      <c r="J1045" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K1045" s="1" t="s">
         <v>91</v>
       </c>
@@ -49704,7 +50008,9 @@
       <c r="I1048" s="1" t="s">
         <v>682</v>
       </c>
-      <c r="J1048" s="1"/>
+      <c r="J1048" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K1048" s="1" t="s">
         <v>91</v>
       </c>
@@ -50462,7 +50768,9 @@
       <c r="I1068" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="J1068" s="1"/>
+      <c r="J1068" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K1068" s="1" t="s">
         <v>91</v>
       </c>
@@ -50916,7 +51224,9 @@
       <c r="I1080" s="1" t="s">
         <v>2545</v>
       </c>
-      <c r="J1080" s="1"/>
+      <c r="J1080" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K1080" s="1" t="s">
         <v>91</v>
       </c>
@@ -50990,7 +51300,9 @@
       <c r="I1082" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="J1082" s="1"/>
+      <c r="J1082" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K1082" s="1" t="s">
         <v>91</v>
       </c>
@@ -51102,7 +51414,9 @@
       <c r="I1085" s="1" t="s">
         <v>2528</v>
       </c>
-      <c r="J1085" s="1"/>
+      <c r="J1085" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K1085" s="1" t="s">
         <v>91</v>
       </c>
@@ -51252,7 +51566,9 @@
       <c r="I1089" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="J1089" s="1"/>
+      <c r="J1089" s="1" t="s">
+        <v>3243</v>
+      </c>
       <c r="K1089" s="1" t="s">
         <v>91</v>
       </c>
@@ -55754,23 +56070,23 @@
       <formula>NOT(ISERROR(SEARCH("""""",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E175:J175 E179:J179 E184:J184 E206:J206 E210:J210 E219:J219 E223:J223 E235:J235 E239:J239 E244:J244 E249:J249 E272:J272 E311:J311 E337:J337 E347:J347 E371:J371 D1:D172 E379:J379 E384:J384 E390:J390 E412:J412 E14:H14 E23:H23 E27:H27 E165:J165 E170:J170 D174:D175 D173:J173 D177:D179 D176:J176 D181:D184 D180:J180 D186:D190 D185:J185 D192:D194 D191:J191 D196:D198 D195:J195 D200:D202 D199:J199 D204:D206 D203:J203 D208:D210 D207:J207 D212 D211:J211 D214 D213:J213 D216:D219 D215:J215 D221:D223 D220:J220 D225:D227 D224:J224 D229:D231 D228:J228 D233:D235 D232:J232 D237:D239 D236:J236 D241:D249 D240:J240 D251:D256 D250:J250 D258:D264 D257:J257 D266:D268 D265:J265 D270:D273 D269:J269 D275:D277 D274:J274 D279:D281 D278:J278 D283:D285 D282:J282 D287:D290 D286:J286 D292:D295 D291:J291 D297:D300 D296:J296 D303:D306 D301:J302 D308:D311 D307:J307 D313:D320 D312:J312 D322:D324 D321:J321 D326:D328 D325:J325 D330:D333 D329:J329 D335:D337 D334:J334 D339:D343 D338:J338 D345:D347 D344:J344 D349:D352 D348:J348 D354:D356 D353:J353 D358:D371 D357:J357 D373:D375 D372:J372 D377:D379 D376:J376 D381:D384 D380:J380 D386:D395 D385:J385 D397:D399 D396:J396 D401:D407 D400:J400 D409:D412 D408:J408 D413:J413 D414:D1048576 E2:L2">
-    <cfRule type="containsBlanks" dxfId="3" priority="2">
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="containsBlanks" dxfId="3" priority="1">
+      <formula>LEN(TRIM(C1))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D172 E2:L2 E14:H14 E23:H23 E27:H27 E165:J165 E170:J170 D173:J173 D174:D175 E175:J175 D176:J176 D177:D179 E179:J179 D180:J180 D181:D184 E184:J184 D185:J185 D186:D190 D191:J191 D192:D194 D195:J195 D196:D198 D199:J199 D200:D202 D203:J203 D204:D206 E206:J206 D207:J207 D208:D210 E210:J210 D211:J211 D212 D213:J213 D214 D215:J215 D216:D219 E219:J219 D220:J220 D221:D223 E223:J223 D224:J224 D225:D227 D228:J228 D229:D231 D232:J232 D233:D235 E235:J235 D236:J236 D237:D239 E239:J239 D240:J240 D241:D249 E244:J244 E249:J249 D250:J250 D251:D256 D257:J257 D258:D264 D265:J265 D266:D268 D269:J269 D270:D273 E272:J272 D274:J274 D275:D277 D278:J278 D279:D281 D282:J282 D283:D285 D286:J286 D287:D290 D291:J291 D292:D295 D296:J296 D297:D300 D301:J302 D303:D306 D307:J307 D308:D311 E311:J311 D312:J312 D313:D320 D321:J321 D322:D324 D325:J325 D326:D328 D329:J329 D330:D333 D334:J334 D335:D337 E337:J337 D338:J338 D339:D343 D344:J344 D345:D347 E347:J347 D348:J348 D349:D352 D353:J353 D354:D356 D357:J357 D358:D371 E371:J371 D372:J372 D373:D375 D376:J376 D377:D379 E379:J379 D380:J380 D381:D384 E384:J384 D385:J385 D386:D395 E390:J390 D396:J396 D397:D399 D400:J400 D401:D407 D408:J408 D409:D412 E412:J412 D413:J413 D414:D1048576">
+    <cfRule type="containsBlanks" dxfId="2" priority="2">
       <formula>LEN(TRIM(D1))=0</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="4">
       <formula>LEN(TRIM(D1))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>""""""</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="6" operator="containsText" text="&quot;&quot;$D$26">
+    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="&quot;&quot;$D$26">
       <formula>NOT(ISERROR(SEARCH("""""$D$26",D1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(C1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Version finale de 2026 avant le peaufinement du code
</commit_message>
<xml_diff>
--- a/BASE_PERSONNEL_.xlsx
+++ b/BASE_PERSONNEL_.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A6B5AA-7F89-4FC9-BDBA-19CCB3F8118C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{66A6B5AA-7F89-4FC9-BDBA-19CCB3F8118C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECA2A2BC-F58F-4A0D-BE5E-F2D18AD2121C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10181,8 +10181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L1207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1197" workbookViewId="0">
-      <selection activeCell="D1205" sqref="D1205"/>
+    <sheetView tabSelected="1" topLeftCell="C92" workbookViewId="0">
+      <selection activeCell="I102" sqref="I102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -56075,7 +56075,7 @@
       <formula>LEN(TRIM(C1))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D172 E2:L2 E14:H14 E23:H23 E27:H27 E165:J165 E170:J170 D173:J173 D174:D175 E175:J175 D176:J176 D177:D179 E179:J179 D180:J180 D181:D184 E184:J184 D185:J185 D186:D190 D191:J191 D192:D194 D195:J195 D196:D198 D199:J199 D200:D202 D203:J203 D204:D206 E206:J206 D207:J207 D208:D210 E210:J210 D211:J211 D212 D213:J213 D214 D215:J215 D216:D219 E219:J219 D220:J220 D221:D223 E223:J223 D224:J224 D225:D227 D228:J228 D229:D231 D232:J232 D233:D235 E235:J235 D236:J236 D237:D239 E239:J239 D240:J240 D241:D249 E244:J244 E249:J249 D250:J250 D251:D256 D257:J257 D258:D264 D265:J265 D266:D268 D269:J269 D270:D273 E272:J272 D274:J274 D275:D277 D278:J278 D279:D281 D282:J282 D283:D285 D286:J286 D287:D290 D291:J291 D292:D295 D296:J296 D297:D300 D301:J302 D303:D306 D307:J307 D308:D311 E311:J311 D312:J312 D313:D320 D321:J321 D322:D324 D325:J325 D326:D328 D329:J329 D330:D333 D334:J334 D335:D337 E337:J337 D338:J338 D339:D343 D344:J344 D345:D347 E347:J347 D348:J348 D349:D352 D353:J353 D354:D356 D357:J357 D358:D371 E371:J371 D372:J372 D373:D375 D376:J376 D377:D379 E379:J379 D380:J380 D381:D384 E384:J384 D385:J385 D386:D395 E390:J390 D396:J396 D397:D399 D400:J400 D401:D407 D408:J408 D409:D412 E412:J412 D413:J413 D414:D1048576">
+  <conditionalFormatting sqref="E2:L2 E14:H14 E23:H23 E27:H27 E165:J165 E170:J170 D173:J173 D174:D175 E175:J175 D176:J176 D177:D179 E179:J179 D180:J180 D181:D184 E184:J184 D185:J185 D186:D190 D191:J191 D192:D194 D195:J195 D196:D198 D199:J199 D200:D202 D203:J203 D204:D206 E206:J206 D207:J207 D208:D210 E210:J210 D211:J211 D212 D213:J213 D214 D215:J215 D216:D219 E219:J219 D220:J220 D221:D223 E223:J223 D224:J224 D225:D227 D228:J228 D229:D231 D232:J232 D233:D235 E235:J235 D236:J236 D237:D239 E239:J239 D240:J240 D241:D249 E244:J244 E249:J249 D250:J250 D251:D256 D257:J257 D258:D264 D265:J265 D266:D268 D269:J269 D270:D273 E272:J272 D274:J274 D275:D277 D278:J278 D279:D281 D282:J282 D283:D285 D286:J286 D287:D290 D291:J291 D292:D295 D296:J296 D297:D300 D301:J302 D303:D306 D307:J307 D308:D311 E311:J311 D312:J312 D313:D320 D321:J321 D322:D324 D325:J325 D326:D328 D329:J329 D330:D333 D334:J334 D335:D337 E337:J337 D338:J338 D339:D343 D344:J344 D345:D347 E347:J347 D348:J348 D349:D352 D353:J353 D354:D356 D357:J357 D358:D371 E371:J371 D372:J372 D373:D375 D376:J376 D377:D379 E379:J379 D380:J380 D381:D384 E384:J384 D385:J385 D386:D395 E390:J390 D396:J396 D397:D399 D400:J400 D401:D407 D408:J408 D409:D412 E412:J412 D413:J413 D414:D1048576 D1:D172">
     <cfRule type="containsBlanks" dxfId="2" priority="2">
       <formula>LEN(TRIM(D1))=0</formula>
     </cfRule>

</xml_diff>